<commit_message>
Improving the data loading function
</commit_message>
<xml_diff>
--- a/Szablon.xlsx
+++ b/Szablon.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="3" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -37,8 +37,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,17 +71,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -119,7 +124,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -153,6 +158,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -187,9 +193,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -362,14 +369,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,6 +396,226 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding xlsx in gitignore
</commit_message>
<xml_diff>
--- a/Szablon.xlsx
+++ b/Szablon.xlsx
@@ -373,7 +373,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,13 +400,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -420,39 +420,39 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -460,13 +460,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -480,142 +480,142 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>324</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F8">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="C10">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="C12">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>